<commit_message>
++ update font size file export shipment FCL
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Shipment Overview - FCL.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Shipment Overview - FCL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.an\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.an\Desktop\eFMS\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -416,23 +416,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="12"/>
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -502,28 +502,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -538,12 +520,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,663 +825,683 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AM17" sqref="AM17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="6" width="11.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25" style="1" customWidth="1"/>
-    <col min="10" max="11" width="17.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="54.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="37.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="20" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="24.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" customWidth="1"/>
-    <col min="20" max="21" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.7109375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="26" style="1" customWidth="1"/>
-    <col min="39" max="39" width="22.85546875" style="1" customWidth="1"/>
-    <col min="40" max="40" width="20" style="1" customWidth="1"/>
-    <col min="41" max="41" width="20.7109375" style="1" customWidth="1"/>
-    <col min="42" max="42" width="21.140625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="17.28515625" style="1" customWidth="1"/>
-    <col min="44" max="44" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.28515625" style="1" customWidth="1"/>
-    <col min="47" max="47" width="14.85546875" style="1" customWidth="1"/>
-    <col min="48" max="48" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20" style="3" customWidth="1"/>
+    <col min="5" max="6" width="11.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20" style="3" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="25" style="3" customWidth="1"/>
+    <col min="10" max="11" width="17.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="54.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="46.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="36.5703125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="37.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="20" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="24.85546875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="10" style="3" customWidth="1"/>
+    <col min="20" max="21" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.7109375" style="3" customWidth="1"/>
+    <col min="33" max="33" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26" style="3" customWidth="1"/>
+    <col min="39" max="39" width="22.85546875" style="3" customWidth="1"/>
+    <col min="40" max="40" width="20" style="3" customWidth="1"/>
+    <col min="41" max="41" width="20.7109375" style="3" customWidth="1"/>
+    <col min="42" max="42" width="21.140625" style="3" customWidth="1"/>
+    <col min="43" max="43" width="17.28515625" style="3" customWidth="1"/>
+    <col min="44" max="44" width="25.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.28515625" style="3" customWidth="1"/>
+    <col min="47" max="47" width="14.85546875" style="3" customWidth="1"/>
+    <col min="48" max="48" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="13"/>
-      <c r="AJ7" s="13"/>
-      <c r="AK7" s="13"/>
-      <c r="AL7" s="13"/>
-      <c r="AM7" s="13"/>
-      <c r="AN7" s="13"/>
-      <c r="AO7" s="13"/>
-      <c r="AP7" s="13"/>
-      <c r="AQ7" s="13"/>
-      <c r="AR7" s="13"/>
-      <c r="AS7" s="13"/>
-      <c r="AT7" s="13"/>
-      <c r="AU7" s="13"/>
-      <c r="AV7" s="13"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="18"/>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
-      <c r="AH8" s="18"/>
-      <c r="AI8" s="18"/>
-      <c r="AJ8" s="18"/>
-      <c r="AK8" s="18"/>
-      <c r="AL8" s="18"/>
-      <c r="AM8" s="18"/>
-      <c r="AN8" s="18"/>
-      <c r="AO8" s="18"/>
-      <c r="AP8" s="18"/>
-      <c r="AQ8" s="18"/>
-      <c r="AR8" s="18"/>
-      <c r="AS8" s="18"/>
-      <c r="AT8" s="18"/>
-      <c r="AU8" s="18"/>
-      <c r="AV8" s="18"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="8"/>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="8"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="N9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="O9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="Q9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="R9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S9" s="8" t="s">
+      <c r="S9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="U9" s="8" t="s">
+      <c r="U9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="V9" s="8" t="s">
+      <c r="V9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="W9" s="8" t="s">
+      <c r="W9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="X9" s="8" t="s">
+      <c r="X9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Y9" s="8" t="s">
+      <c r="Y9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Z9" s="8" t="s">
+      <c r="Z9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AA9" s="10" t="s">
+      <c r="AA9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AB9" s="10"/>
-      <c r="AC9" s="10"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
-      <c r="AH9" s="10"/>
-      <c r="AI9" s="10"/>
-      <c r="AJ9" s="10" t="s">
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="11"/>
+      <c r="AH9" s="11"/>
+      <c r="AI9" s="11"/>
+      <c r="AJ9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AK9" s="10" t="s">
+      <c r="AK9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AL9" s="10"/>
-      <c r="AM9" s="10"/>
-      <c r="AN9" s="10"/>
-      <c r="AO9" s="10"/>
-      <c r="AP9" s="10"/>
-      <c r="AQ9" s="10"/>
-      <c r="AR9" s="10"/>
-      <c r="AS9" s="10" t="s">
+      <c r="AL9" s="11"/>
+      <c r="AM9" s="11"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="11"/>
+      <c r="AP9" s="11"/>
+      <c r="AQ9" s="11"/>
+      <c r="AR9" s="11"/>
+      <c r="AS9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AT9" s="10" t="s">
+      <c r="AT9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AU9" s="10" t="s">
+      <c r="AU9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AV9" s="10" t="s">
+      <c r="AV9" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="2" t="s">
+    <row r="10" spans="1:48" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AB10" s="2" t="s">
+      <c r="AB10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AC10" s="2" t="s">
+      <c r="AC10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AD10" s="2" t="s">
+      <c r="AD10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AE10" s="2" t="s">
+      <c r="AE10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AF10" s="2" t="s">
+      <c r="AF10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AG10" s="2" t="s">
+      <c r="AG10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AH10" s="2" t="s">
+      <c r="AH10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AI10" s="3" t="s">
+      <c r="AI10" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AJ10" s="3" t="s">
+      <c r="AJ10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AK10" s="2" t="s">
+      <c r="AK10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AL10" s="2" t="s">
+      <c r="AL10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AM10" s="2" t="s">
+      <c r="AM10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AN10" s="2" t="s">
+      <c r="AN10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AO10" s="2" t="s">
+      <c r="AO10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AP10" s="2" t="s">
+      <c r="AP10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AQ10" s="2" t="s">
+      <c r="AQ10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AR10" s="3" t="s">
+      <c r="AR10" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AS10" s="3" t="s">
+      <c r="AS10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AT10" s="11"/>
-      <c r="AU10" s="11"/>
-      <c r="AV10" s="11"/>
+      <c r="AT10" s="16"/>
+      <c r="AU10" s="16"/>
+      <c r="AV10" s="16"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="S11" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="T11" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="U11" s="4" t="s">
+      <c r="U11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="V11" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="W11" s="4" t="s">
+      <c r="W11" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="X11" s="4" t="s">
+      <c r="X11" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="Y11" s="4" t="s">
+      <c r="Y11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="Z11" s="4" t="s">
+      <c r="Z11" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AA11" s="5" t="s">
+      <c r="AA11" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AB11" s="5" t="s">
+      <c r="AB11" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="AC11" s="5" t="s">
+      <c r="AC11" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="AD11" s="5" t="s">
+      <c r="AD11" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="AE11" s="5" t="s">
+      <c r="AE11" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="AF11" s="5" t="s">
+      <c r="AF11" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="AG11" s="5" t="s">
+      <c r="AG11" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="AH11" s="5" t="s">
+      <c r="AH11" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="AI11" s="5" t="s">
+      <c r="AI11" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="AJ11" s="5" t="s">
+      <c r="AJ11" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="AK11" s="5" t="s">
+      <c r="AK11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="AL11" s="5" t="s">
+      <c r="AL11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AM11" s="5" t="s">
+      <c r="AM11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="AN11" s="5" t="s">
+      <c r="AN11" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="AO11" s="5" t="s">
+      <c r="AO11" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AP11" s="5" t="s">
+      <c r="AP11" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="AQ11" s="5" t="s">
+      <c r="AQ11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="AR11" s="5" t="s">
+      <c r="AR11" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="AS11" s="5" t="s">
+      <c r="AS11" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="AT11" s="6" t="s">
+      <c r="AT11" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="AU11" s="5" t="s">
+      <c r="AU11" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="AV11" s="5" t="s">
+      <c r="AV11" s="18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="7" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="U12" s="7" t="s">
+      <c r="U12" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="V12" s="7" t="s">
+      <c r="V12" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="W12" s="7" t="s">
+      <c r="W12" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="X12" s="7" t="s">
+      <c r="X12" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="Y12" s="7" t="s">
+      <c r="Y12" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="Z12" s="7" t="s">
+      <c r="Z12" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="AA12" s="5" t="s">
+      <c r="AA12" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="AB12" s="5" t="s">
+      <c r="AB12" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="AC12" s="5" t="s">
+      <c r="AC12" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="AD12" s="5" t="s">
+      <c r="AD12" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="AE12" s="5" t="s">
+      <c r="AE12" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="AF12" s="5" t="s">
+      <c r="AF12" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="AG12" s="5" t="s">
+      <c r="AG12" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="AH12" s="5" t="s">
+      <c r="AH12" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="AI12" s="5" t="s">
+      <c r="AI12" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="AJ12" s="5" t="s">
+      <c r="AJ12" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="AK12" s="5" t="s">
+      <c r="AK12" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="AL12" s="5" t="s">
+      <c r="AL12" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="AM12" s="5" t="s">
+      <c r="AM12" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="AN12" s="5" t="s">
+      <c r="AN12" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="AO12" s="5" t="s">
+      <c r="AO12" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="AP12" s="5" t="s">
+      <c r="AP12" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="AQ12" s="5" t="s">
+      <c r="AQ12" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="AR12" s="5" t="s">
+      <c r="AR12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="AS12" s="5" t="s">
+      <c r="AS12" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="AT12" s="5" t="s">
+      <c r="AT12" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="AU12" s="5" t="s">
+      <c r="AU12" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="AV12" s="5" t="s">
+      <c r="AV12" s="18" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D6"/>
+    <mergeCell ref="A7:AV7"/>
+    <mergeCell ref="A8:AV8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
     <mergeCell ref="A12:S12"/>
     <mergeCell ref="Y9:Y10"/>
     <mergeCell ref="Z9:Z10"/>
@@ -1499,26 +1518,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D6"/>
-    <mergeCell ref="A7:AV7"/>
-    <mergeCell ref="A8:AV8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
++ update copy file
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Shipment Overview - FCL.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Shipment Overview - FCL.xlsx
@@ -504,8 +504,25 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -520,29 +537,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,682 +826,662 @@
   <dimension ref="A1:AV12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="20" style="3" customWidth="1"/>
-    <col min="5" max="6" width="11.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20" style="3" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="25" style="3" customWidth="1"/>
-    <col min="10" max="11" width="17.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="54.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="46.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="36.5703125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="37.140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="20" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="24.85546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="10" style="3" customWidth="1"/>
-    <col min="20" max="21" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.7109375" style="3" customWidth="1"/>
-    <col min="33" max="33" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="26" style="3" customWidth="1"/>
-    <col min="39" max="39" width="22.85546875" style="3" customWidth="1"/>
-    <col min="40" max="40" width="20" style="3" customWidth="1"/>
-    <col min="41" max="41" width="20.7109375" style="3" customWidth="1"/>
-    <col min="42" max="42" width="21.140625" style="3" customWidth="1"/>
-    <col min="43" max="43" width="17.28515625" style="3" customWidth="1"/>
-    <col min="44" max="44" width="25.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.28515625" style="3" customWidth="1"/>
-    <col min="47" max="47" width="14.85546875" style="3" customWidth="1"/>
-    <col min="48" max="48" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="6" width="11.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25" style="1" customWidth="1"/>
+    <col min="10" max="11" width="17.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="54.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="46.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="36.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="37.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="24.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10" style="1" customWidth="1"/>
+    <col min="20" max="21" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.7109375" style="1" customWidth="1"/>
+    <col min="33" max="33" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26" style="1" customWidth="1"/>
+    <col min="39" max="39" width="22.85546875" style="1" customWidth="1"/>
+    <col min="40" max="40" width="20" style="1" customWidth="1"/>
+    <col min="41" max="41" width="20.7109375" style="1" customWidth="1"/>
+    <col min="42" max="42" width="21.140625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="17.28515625" style="1" customWidth="1"/>
+    <col min="44" max="44" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.28515625" style="1" customWidth="1"/>
+    <col min="47" max="47" width="14.85546875" style="1" customWidth="1"/>
+    <col min="48" max="48" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
-      <c r="AO7" s="2"/>
-      <c r="AP7" s="2"/>
-      <c r="AQ7" s="2"/>
-      <c r="AR7" s="2"/>
-      <c r="AS7" s="2"/>
-      <c r="AT7" s="2"/>
-      <c r="AU7" s="2"/>
-      <c r="AV7" s="2"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="12"/>
+      <c r="AG7" s="12"/>
+      <c r="AH7" s="12"/>
+      <c r="AI7" s="12"/>
+      <c r="AJ7" s="12"/>
+      <c r="AK7" s="12"/>
+      <c r="AL7" s="12"/>
+      <c r="AM7" s="12"/>
+      <c r="AN7" s="12"/>
+      <c r="AO7" s="12"/>
+      <c r="AP7" s="12"/>
+      <c r="AQ7" s="12"/>
+      <c r="AR7" s="12"/>
+      <c r="AS7" s="12"/>
+      <c r="AT7" s="12"/>
+      <c r="AU7" s="12"/>
+      <c r="AV7" s="12"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="8"/>
-      <c r="AN8" s="8"/>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
-      <c r="AR8" s="8"/>
-      <c r="AS8" s="8"/>
-      <c r="AT8" s="8"/>
-      <c r="AU8" s="8"/>
-      <c r="AV8" s="8"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="17"/>
+      <c r="AG8" s="17"/>
+      <c r="AH8" s="17"/>
+      <c r="AI8" s="17"/>
+      <c r="AJ8" s="17"/>
+      <c r="AK8" s="17"/>
+      <c r="AL8" s="17"/>
+      <c r="AM8" s="17"/>
+      <c r="AN8" s="17"/>
+      <c r="AO8" s="17"/>
+      <c r="AP8" s="17"/>
+      <c r="AQ8" s="17"/>
+      <c r="AR8" s="17"/>
+      <c r="AS8" s="17"/>
+      <c r="AT8" s="17"/>
+      <c r="AU8" s="17"/>
+      <c r="AV8" s="17"/>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="P9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="S9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="T9" s="9" t="s">
+      <c r="T9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="U9" s="9" t="s">
+      <c r="U9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V9" s="9" t="s">
+      <c r="V9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="W9" s="9" t="s">
+      <c r="W9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="X9" s="9" t="s">
+      <c r="X9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Y9" s="9" t="s">
+      <c r="Y9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Z9" s="9" t="s">
+      <c r="Z9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AA9" s="11" t="s">
+      <c r="AA9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11"/>
-      <c r="AH9" s="11"/>
-      <c r="AI9" s="11"/>
-      <c r="AJ9" s="11" t="s">
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AK9" s="11" t="s">
+      <c r="AK9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AL9" s="11"/>
-      <c r="AM9" s="11"/>
-      <c r="AN9" s="11"/>
-      <c r="AO9" s="11"/>
-      <c r="AP9" s="11"/>
-      <c r="AQ9" s="11"/>
-      <c r="AR9" s="11"/>
-      <c r="AS9" s="11" t="s">
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AT9" s="11" t="s">
+      <c r="AT9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AU9" s="11" t="s">
+      <c r="AU9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AV9" s="11" t="s">
+      <c r="AV9" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:48" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="14" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AB10" s="14" t="s">
+      <c r="AB10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC10" s="14" t="s">
+      <c r="AC10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AD10" s="14" t="s">
+      <c r="AD10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AE10" s="14" t="s">
+      <c r="AE10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AF10" s="14" t="s">
+      <c r="AF10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AG10" s="14" t="s">
+      <c r="AG10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AH10" s="14" t="s">
+      <c r="AH10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AI10" s="15" t="s">
+      <c r="AI10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AJ10" s="15" t="s">
+      <c r="AJ10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AK10" s="14" t="s">
+      <c r="AK10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AL10" s="14" t="s">
+      <c r="AL10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AM10" s="14" t="s">
+      <c r="AM10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AN10" s="14" t="s">
+      <c r="AN10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AO10" s="14" t="s">
+      <c r="AO10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AP10" s="14" t="s">
+      <c r="AP10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AQ10" s="14" t="s">
+      <c r="AQ10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AR10" s="15" t="s">
+      <c r="AR10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AS10" s="15" t="s">
+      <c r="AS10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AT10" s="16"/>
-      <c r="AU10" s="16"/>
-      <c r="AV10" s="16"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
+      <c r="AV10" s="10"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="17" t="s">
+      <c r="N11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="17" t="s">
+      <c r="O11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="Q11" s="17" t="s">
+      <c r="Q11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="R11" s="17" t="s">
+      <c r="R11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="S11" s="17" t="s">
+      <c r="S11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="T11" s="17" t="s">
+      <c r="T11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="U11" s="17" t="s">
+      <c r="U11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="V11" s="17" t="s">
+      <c r="V11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="W11" s="17" t="s">
+      <c r="W11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="X11" s="17" t="s">
+      <c r="X11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="Y11" s="17" t="s">
+      <c r="Y11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Z11" s="17" t="s">
+      <c r="Z11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AA11" s="18" t="s">
+      <c r="AA11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AB11" s="18" t="s">
+      <c r="AB11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AC11" s="18" t="s">
+      <c r="AC11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AD11" s="18" t="s">
+      <c r="AD11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AE11" s="18" t="s">
+      <c r="AE11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AF11" s="18" t="s">
+      <c r="AF11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AG11" s="18" t="s">
+      <c r="AG11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AH11" s="18" t="s">
+      <c r="AH11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AI11" s="18" t="s">
+      <c r="AI11" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AJ11" s="18" t="s">
+      <c r="AJ11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AK11" s="18" t="s">
+      <c r="AK11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AL11" s="18" t="s">
+      <c r="AL11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AM11" s="18" t="s">
+      <c r="AM11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AN11" s="18" t="s">
+      <c r="AN11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AO11" s="18" t="s">
+      <c r="AO11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AP11" s="18" t="s">
+      <c r="AP11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AQ11" s="18" t="s">
+      <c r="AQ11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="AR11" s="18" t="s">
+      <c r="AR11" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="AS11" s="18" t="s">
+      <c r="AS11" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AT11" s="19" t="s">
+      <c r="AT11" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AU11" s="18" t="s">
+      <c r="AU11" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AV11" s="18" t="s">
+      <c r="AV11" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="17" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="U12" s="17" t="s">
+      <c r="U12" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="V12" s="17" t="s">
+      <c r="V12" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="W12" s="17" t="s">
+      <c r="W12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="X12" s="17" t="s">
+      <c r="X12" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Y12" s="17" t="s">
+      <c r="Y12" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="Z12" s="17" t="s">
+      <c r="Z12" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="AA12" s="18" t="s">
+      <c r="AA12" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AB12" s="18" t="s">
+      <c r="AB12" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="AC12" s="18" t="s">
+      <c r="AC12" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="AD12" s="18" t="s">
+      <c r="AD12" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="AE12" s="18" t="s">
+      <c r="AE12" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="AF12" s="18" t="s">
+      <c r="AF12" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="AG12" s="18" t="s">
+      <c r="AG12" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="AH12" s="18" t="s">
+      <c r="AH12" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AI12" s="18" t="s">
+      <c r="AI12" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="AJ12" s="18" t="s">
+      <c r="AJ12" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="AK12" s="18" t="s">
+      <c r="AK12" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="AL12" s="18" t="s">
+      <c r="AL12" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="AM12" s="18" t="s">
+      <c r="AM12" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="AN12" s="18" t="s">
+      <c r="AN12" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="AO12" s="18" t="s">
+      <c r="AO12" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AP12" s="18" t="s">
+      <c r="AP12" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="AQ12" s="18" t="s">
+      <c r="AQ12" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="AR12" s="18" t="s">
+      <c r="AR12" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="AS12" s="18" t="s">
+      <c r="AS12" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="AT12" s="18" t="s">
+      <c r="AT12" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="AU12" s="18" t="s">
+      <c r="AU12" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AV12" s="18" t="s">
+      <c r="AV12" s="5" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D6"/>
-    <mergeCell ref="A7:AV7"/>
-    <mergeCell ref="A8:AV8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
     <mergeCell ref="A12:S12"/>
     <mergeCell ref="Y9:Y10"/>
     <mergeCell ref="Z9:Z10"/>
@@ -1518,6 +1498,26 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D6"/>
+    <mergeCell ref="A7:AV7"/>
+    <mergeCell ref="A8:AV8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>